<commit_message>
add: undifined.py write style
</commit_message>
<xml_diff>
--- a/dev_data.xlsx
+++ b/dev_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3435" windowWidth="20325" windowHeight="8640" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="3795" windowWidth="20325" windowHeight="8640"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="125">
   <si>
     <t>Hostname</t>
   </si>
@@ -159,27 +159,6 @@
   </si>
   <si>
     <t>show run int vlan 2</t>
-  </si>
-  <si>
-    <t>#</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -235,39 +214,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>H</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>uawei@123</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>huawei</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.56.10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.56.20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.56.30</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>display vlan s</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -419,22 +365,160 @@
     <t>config_command_15</t>
   </si>
   <si>
-    <t>#</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>sysn SW1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>sysn SW2</t>
-  </si>
-  <si>
-    <t>sysn SW3</t>
-  </si>
-  <si>
-    <t>192.168.56.111</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>10.88.254.1</t>
+  </si>
+  <si>
+    <t>10.88.254.2</t>
+  </si>
+  <si>
+    <t>10.88.254.3</t>
+  </si>
+  <si>
+    <t>10.88.254.4</t>
+  </si>
+  <si>
+    <t>10.88.254.5</t>
+  </si>
+  <si>
+    <t>10.88.254.6</t>
+  </si>
+  <si>
+    <t>10.88.254.7</t>
+  </si>
+  <si>
+    <t>10.88.254.8</t>
+  </si>
+  <si>
+    <t>10.88.254.9</t>
+  </si>
+  <si>
+    <t>10.88.254.10</t>
+  </si>
+  <si>
+    <t>10.88.254.11</t>
+  </si>
+  <si>
+    <t>10.88.254.12</t>
+  </si>
+  <si>
+    <t>10.88.254.13</t>
+  </si>
+  <si>
+    <t>10.88.254.14</t>
+  </si>
+  <si>
+    <t>10.88.254.15</t>
+  </si>
+  <si>
+    <t>10.88.254.16</t>
+  </si>
+  <si>
+    <t>10.88.254.17</t>
+  </si>
+  <si>
+    <t>10.88.254.18</t>
+  </si>
+  <si>
+    <t>10.88.254.254</t>
+  </si>
+  <si>
+    <t>10.88.253.1</t>
+  </si>
+  <si>
+    <t>10.88.253.2</t>
+  </si>
+  <si>
+    <t>10.88.253.3</t>
+  </si>
+  <si>
+    <t>10.88.253.4</t>
+  </si>
+  <si>
+    <t>10.88.253.5</t>
+  </si>
+  <si>
+    <t>10.88.253.6</t>
+  </si>
+  <si>
+    <t>10.88.253.7</t>
+  </si>
+  <si>
+    <t>10.88.253.8</t>
+  </si>
+  <si>
+    <t>10.88.253.9</t>
+  </si>
+  <si>
+    <t>10.88.253.10</t>
+  </si>
+  <si>
+    <t>10.88.253.11</t>
+  </si>
+  <si>
+    <t>10.88.253.12</t>
+  </si>
+  <si>
+    <t>10.88.253.13</t>
+  </si>
+  <si>
+    <t>10.88.253.14</t>
+  </si>
+  <si>
+    <t>10.88.253.15</t>
+  </si>
+  <si>
+    <t>10.88.253.16</t>
+  </si>
+  <si>
+    <t>10.88.253.17</t>
+  </si>
+  <si>
+    <t>10.88.253.18</t>
+  </si>
+  <si>
+    <t>10.88.253.19</t>
+  </si>
+  <si>
+    <t>10.88.253.20</t>
+  </si>
+  <si>
+    <t>10.88.253.21</t>
+  </si>
+  <si>
+    <t>10.88.253.22</t>
+  </si>
+  <si>
+    <t>10.88.253.23</t>
+  </si>
+  <si>
+    <t>10.88.253.24</t>
+  </si>
+  <si>
+    <t>10.88.253.25</t>
+  </si>
+  <si>
+    <t>10.88.253.26</t>
+  </si>
+  <si>
+    <t>10.88.253.27</t>
+  </si>
+  <si>
+    <t>10.88.253.28</t>
+  </si>
+  <si>
+    <t>10.88.253.29</t>
+  </si>
+  <si>
+    <t>10.88.253.30</t>
+  </si>
+  <si>
+    <t>10.88.253.254</t>
+  </si>
+  <si>
+    <t>h3c@20230630</t>
+  </si>
+  <si>
+    <t>hp_comware</t>
   </si>
 </sst>
 </file>
@@ -896,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -931,10 +1015,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>5</v>
@@ -944,77 +1028,855 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="8"/>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>51</v>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" t="s">
+        <v>123</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s">
+        <v>123</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s">
+        <v>123</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" t="s">
+        <v>123</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" t="s">
+        <v>123</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" t="s">
+        <v>123</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
+        <v>123</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
+        <v>123</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" t="s">
+        <v>123</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
+        <v>123</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1044,10 +1906,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -1056,7 +1918,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -1065,7 +1927,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -1074,25 +1936,25 @@
         <v>15</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -1105,7 +1967,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4"/>
     </row>
@@ -1770,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1810,10 +2672,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>5</v>
@@ -1822,73 +2684,69 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C2" t="s">
         <v>73</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="C2" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
@@ -1898,27 +2756,23 @@
       <c r="R2" s="11"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="C3" s="9" t="s">
-        <v>53</v>
+      <c r="C3" t="s">
+        <v>74</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
@@ -1928,27 +2782,23 @@
       <c r="R3" s="11"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="C4" s="9" t="s">
-        <v>54</v>
+      <c r="C4" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
@@ -1957,6 +2807,805 @@
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
     </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" t="s">
+        <v>123</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s">
+        <v>123</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s">
+        <v>123</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" t="s">
+        <v>123</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" t="s">
+        <v>123</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C42" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" t="s">
+        <v>123</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
+        <v>123</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
+        <v>123</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" t="s">
+        <v>123</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.15">
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
+        <v>123</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>